<commit_message>
Adicionado Script de criação de usuarios e privilegios
</commit_message>
<xml_diff>
--- a/controle de acesso.xlsx
+++ b/controle de acesso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitall\bancodedados\insideprovider\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262E57C6-425E-4891-B1D7-4C03F2D54BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4F0A97-576E-4787-8ED0-5126453C0A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Financeiro</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>A-V</t>
-  </si>
-  <si>
-    <t>C-A</t>
   </si>
   <si>
     <t>Administrador</t>
@@ -149,13 +146,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,7 +436,7 @@
   <dimension ref="C6:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,12 +449,12 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
@@ -476,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.25">
@@ -526,7 +523,7 @@
       <c r="E10" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -558,7 +555,7 @@
       <c r="I11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
@@ -591,7 +588,7 @@
         <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>1</v>
@@ -615,7 +612,7 @@
       </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="G15" s="4"/>
+      <c r="G15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>